<commit_message>
Actualizacion - Semana 7
</commit_message>
<xml_diff>
--- a/Produccion.xlsx
+++ b/Produccion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41291a4e6da63335/Documentos/8vo semestre/Tesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{02B0CECB-CD3F-4B82-9A7D-64C2BB3535D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5608BFB-4114-4343-8363-61D8479AA3FB}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{02B0CECB-CD3F-4B82-9A7D-64C2BB3535D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEA776D1-A0E9-460B-ABC6-B99F89FC52A5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{EEBEEA34-E90F-4518-AB25-F2FEA12A11A5}"/>
+    <workbookView minimized="1" xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7785" xr2:uid="{EEBEEA34-E90F-4518-AB25-F2FEA12A11A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Produccion" sheetId="3" r:id="rId1"/>
@@ -708,20 +708,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E5C3F7-D832-4B21-A40F-B36A5D6353C6}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -765,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1982</v>
       </c>
@@ -809,7 +809,7 @@
         <v>33721</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1983</v>
       </c>
@@ -853,7 +853,7 @@
         <v>36150</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>1984</v>
       </c>
@@ -897,7 +897,7 @@
         <v>39152</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>1985</v>
       </c>
@@ -941,7 +941,7 @@
         <v>42610</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>1986</v>
       </c>
@@ -985,7 +985,7 @@
         <v>45621</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>1987</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>44882</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>1988</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>45802</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>1989</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>46270</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>1990</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>50372</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>1991</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>51599</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>1992</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>46528</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>1993</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>54004</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1994</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>48900</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>1995</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>47552</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>1996</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>40838</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>1997</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>38604</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>1998</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>39487.480900000002</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>1999</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>34863.754150000001</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2000</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>36730.771919999999</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>2001</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>36070.202100000002</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>2002</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>34001.953259999995</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>2003</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>41704.519650000002</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>2004</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>36356</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>2005</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>37909.314539999999</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>2006</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>30357.358209999999</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>2007</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>33478.5</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>2008</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>37719.089719999996</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>2009</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>36118</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>2010</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>42294.5645</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>2011</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>37202</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>2012</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>41671</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>2013</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>46738.883800000003</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>2014</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>2015</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>54797.950680000002</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>2016</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>56762</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>2017</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>60535</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>2018</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>97978</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>2019</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>102154</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>2020</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>63416</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>2021</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>69040</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>2022</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>62158</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>2023</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>59831</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
         <v>2024</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>67678</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="19">
         <v>2025</v>
       </c>
@@ -2719,16 +2719,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42026199-1B64-4D63-B428-C4FFDF5F7BE0}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A17" zoomScale="77" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1982</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1983</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>1984</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>1985</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>1986</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>1987</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>1988</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>1989</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>1990</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>1991</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>1992</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>1993</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1994</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>1995</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>1996</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>1997</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>1998</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>1999</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2000</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>2001</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>2002</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>2003</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>2004</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>2005</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>2006</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>2007</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>2008</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>2009</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>2010</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>2011</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>2012</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>2013</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>2014</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>2015</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>2016</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>2017</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B39" s="17">
         <f>AVERAGE(B2:B37)</f>
         <v>0.10336369506742837</v>

</xml_diff>